<commit_message>
add search for students:
</commit_message>
<xml_diff>
--- a/static/excel/studentswithmajor.xlsx
+++ b/static/excel/studentswithmajor.xlsx
@@ -286,7 +286,7 @@
     <t>ماريا نائل عيسى</t>
   </si>
   <si>
-    <t>رأفت ماجد كريشي</t>
+    <t>رأفت ماجد كريش</t>
   </si>
   <si>
     <t>عبد الاله أيمن طالب</t>
@@ -828,7 +828,7 @@
     <col min="3" max="3" style="13" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>